<commit_message>
Added local and distributed witness files
</commit_message>
<xml_diff>
--- a/Verify_comm100.xlsx
+++ b/Verify_comm100.xlsx
@@ -450,13 +450,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.447177</v>
+        <v>0.298981</v>
       </c>
       <c r="C2" t="n">
-        <v>1.569629</v>
+        <v>8.685805</v>
       </c>
       <c r="D2" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>